<commit_message>
Adding autocomplete guide for Django in Atom IDE
</commit_message>
<xml_diff>
--- a/COMMANDS.xlsx
+++ b/COMMANDS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Administration</t>
   </si>
@@ -127,6 +127,37 @@
   </si>
   <si>
     <t>python manage.py migrate</t>
+  </si>
+  <si>
+    <t>Atom autocomplete:</t>
+  </si>
+  <si>
+    <t>1. Search for "autocomplete-python" and click "Install"</t>
+  </si>
+  <si>
+    <t>2. Go to the packages Settings (in the Packages section of Atom's settings)</t>
+  </si>
+  <si>
+    <t>3. Enter the path to your virtualenv's site-packages dir in the Extra PATH setting.</t>
+  </si>
+  <si>
+    <t>4. Restart Atom</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for example:  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C:\Users\georgivelikov\anaconda3\envs\myDjangoEnv\Lib\site-packages</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -244,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -257,6 +288,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F36"/>
+  <dimension ref="B1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,43 +785,55 @@
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
+      <c r="B23" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="B24" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
+      <c r="B25" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="E25" s="3"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
+      <c r="B26" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="E26" s="3"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
+      <c r="B27" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="E27" s="3"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
+      <c r="B28" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="E28" s="3"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="E29" s="3"/>
       <c r="F29" s="2"/>
@@ -830,11 +874,17 @@
       <c r="E35" s="3"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>